<commit_message>
added steelhead LGR figure
</commit_message>
<xml_diff>
--- a/data/input/mgt_targets.xlsx
+++ b/data/input/mgt_targets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nezperce365-my.sharepoint.com/personal/ryank_nezperce_org/Documents/Projects/DFRM Research Division/Abundance_Declines/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SRAFS\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="305" documentId="13_ncr:1_{3F550AED-EFB5-463C-AD04-90F20DD3C7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A06FD472-6442-4C90-8F73-D7DA563BCB5C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2362FA7-A0BC-44A2-A206-98358A0DD00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8955" yWindow="885" windowWidth="38625" windowHeight="17820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goals and Thresholds" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="107">
   <si>
     <t xml:space="preserve">Total </t>
   </si>
@@ -1277,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="D29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,25 +1320,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>76</v>
       </c>
       <c r="F2">
-        <v>325000</v>
-      </c>
-      <c r="G2" t="s">
-        <v>81</v>
+        <v>4400</v>
       </c>
       <c r="H2" t="s">
         <v>39</v>
@@ -1346,51 +1343,45 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F3">
-        <v>235000</v>
-      </c>
-      <c r="G3" t="s">
-        <v>82</v>
+        <v>2147</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>76</v>
       </c>
       <c r="F4">
-        <v>90000</v>
-      </c>
-      <c r="G4" t="s">
-        <v>83</v>
+        <v>48500</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
@@ -1398,36 +1389,36 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="F5">
-        <v>277400</v>
+        <v>250</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1436,7 +1427,7 @@
         <v>76</v>
       </c>
       <c r="F6">
-        <v>147300</v>
+        <v>44100</v>
       </c>
       <c r="H6" t="s">
         <v>39</v>
@@ -1444,48 +1435,48 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7">
-        <v>130100</v>
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8">
-        <v>43000</v>
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1499,13 +1490,13 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
         <v>76</v>
       </c>
       <c r="F9">
-        <v>18200</v>
+        <v>24800</v>
       </c>
       <c r="H9" t="s">
         <v>39</v>
@@ -1525,24 +1516,24 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F10">
-        <v>24800</v>
+        <v>3614</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1551,7 +1542,7 @@
         <v>76</v>
       </c>
       <c r="F11">
-        <v>48500</v>
+        <v>43000</v>
       </c>
       <c r="H11" t="s">
         <v>39</v>
@@ -1559,45 +1550,45 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="F12">
-        <v>44100</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
         <v>76</v>
       </c>
       <c r="F13">
-        <v>4400</v>
+        <v>18200</v>
       </c>
       <c r="H13" t="s">
         <v>39</v>
@@ -1605,48 +1596,48 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F14">
-        <v>54600</v>
+        <v>5300</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F15">
-        <v>54600</v>
+        <v>11700</v>
       </c>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1674,82 +1665,79 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>78</v>
       </c>
       <c r="F17">
-        <v>43000</v>
-      </c>
-      <c r="G17" t="s">
-        <v>86</v>
+        <v>1183</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F18">
-        <v>30800</v>
+        <v>54600</v>
       </c>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="F19">
-        <v>5300</v>
+        <v>450</v>
       </c>
       <c r="H19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1758,13 +1746,13 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" t="s">
-        <v>10</v>
+        <v>76</v>
+      </c>
+      <c r="F20">
+        <v>54600</v>
       </c>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,28 +1780,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="F22">
-        <v>1850</v>
-      </c>
-      <c r="G22" t="s">
-        <v>41</v>
+        <v>33100</v>
       </c>
       <c r="H22" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1830,36 +1815,39 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F23">
-        <v>11638</v>
+        <v>90000</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F24">
-        <v>1200</v>
+        <v>11638</v>
+      </c>
+      <c r="G24" t="s">
+        <v>84</v>
       </c>
       <c r="H24" t="s">
         <v>37</v>
@@ -1867,36 +1855,39 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F25">
-        <v>5285</v>
+        <v>325000</v>
+      </c>
+      <c r="G25" t="s">
+        <v>81</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -1905,7 +1896,10 @@
         <v>41</v>
       </c>
       <c r="F26">
-        <v>50</v>
+        <v>1850</v>
+      </c>
+      <c r="G26" t="s">
+        <v>41</v>
       </c>
       <c r="H26" t="s">
         <v>37</v>
@@ -1913,105 +1907,117 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F27">
-        <v>3614</v>
+        <v>235000</v>
+      </c>
+      <c r="G27" t="s">
+        <v>82</v>
       </c>
       <c r="H27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F28">
-        <v>250</v>
+        <v>43000</v>
+      </c>
+      <c r="G28" t="s">
+        <v>86</v>
       </c>
       <c r="H28" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F29">
-        <v>2147</v>
+        <v>137000</v>
+      </c>
+      <c r="G29" t="s">
+        <v>85</v>
       </c>
       <c r="H29" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="F30">
-        <v>450</v>
+        <v>130100</v>
+      </c>
+      <c r="G30" t="s">
+        <v>83</v>
       </c>
       <c r="H30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -2020,7 +2026,10 @@
         <v>78</v>
       </c>
       <c r="F31">
-        <v>1183</v>
+        <v>5285</v>
+      </c>
+      <c r="G31" t="s">
+        <v>84</v>
       </c>
       <c r="H31" t="s">
         <v>37</v>
@@ -2028,28 +2037,28 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F32">
-        <v>137000</v>
+        <v>277400</v>
       </c>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2066,56 +2075,65 @@
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F33">
-        <v>83200</v>
+        <v>1200</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
       </c>
       <c r="H33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F34">
-        <v>11700</v>
+        <v>147300</v>
+      </c>
+      <c r="G34" t="s">
+        <v>82</v>
       </c>
       <c r="H34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F35" t="s">
-        <v>10</v>
+        <v>78</v>
+      </c>
+      <c r="F35">
+        <v>30800</v>
+      </c>
+      <c r="G35" t="s">
+        <v>86</v>
       </c>
       <c r="H35" t="s">
         <v>40</v>
@@ -2123,13 +2141,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -2138,13 +2156,21 @@
         <v>77</v>
       </c>
       <c r="F36">
-        <v>33100</v>
+        <v>83200</v>
+      </c>
+      <c r="G36" t="s">
+        <v>85</v>
       </c>
       <c r="H36" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H36">
+    <sortCondition ref="A2:A36"/>
+    <sortCondition ref="D2:D36"/>
+    <sortCondition ref="E2:E36"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2154,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="G275" sqref="G275"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>